<commit_message>
Neues Burndown Chart mit Daten vom 14.03.2024
</commit_message>
<xml_diff>
--- a/Burndown Chart STMX Shop.xlsx
+++ b/Burndown Chart STMX Shop.xlsx
@@ -1,31 +1,43 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27511"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Desktop\CTS\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{6A744AAC-1D38-491D-A017-BF33ACFDC779}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11850" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11850" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle2" sheetId="2" r:id="rId1"/>
     <sheet name="Tabelle1" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
   <si>
     <t>Grundgerüst HTML Startseite</t>
   </si>
@@ -118,13 +130,19 @@
   </si>
   <si>
     <t>Footer auf Supportseite</t>
+  </si>
+  <si>
+    <t>Support Seite</t>
+  </si>
+  <si>
+    <t>Letzte Bugfixes</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -214,7 +232,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -240,7 +257,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="de-DE"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -264,10 +281,10 @@
           </c:spPr>
           <c:cat>
             <c:numRef>
-              <c:f>Tabelle1!$C$1:$C$11</c:f>
+              <c:f>Tabelle1!$C$1:$C$12</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>45320</c:v>
                 </c:pt>
@@ -300,47 +317,53 @@
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>45362</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>45365</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Tabelle1!$E$1:$E$11</c:f>
+              <c:f>Tabelle1!$E$1:$E$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>29</c:v>
+                  <c:v>31</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>24</c:v>
+                  <c:v>26</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>20</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>17</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>16</c:v>
                 </c:pt>
-                <c:pt idx="5">
-                  <c:v>14</c:v>
-                </c:pt>
                 <c:pt idx="6">
-                  <c:v>11</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>8</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>4</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="10">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="11">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -404,7 +427,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="879181120"/>
@@ -462,7 +485,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="879178824"/>
@@ -503,7 +526,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="de-DE"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1079,20 +1102,26 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>4581525</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>161925</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>523875</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="6" name="Diagramm 5"/>
+        <xdr:cNvPr id="6" name="Diagramm 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000006000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -1372,34 +1401,34 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E31"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:E33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="K26" sqref="K26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="15.42578125" customWidth="1"/>
     <col min="2" max="2" width="96.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1" s="1">
         <v>45320</v>
       </c>
@@ -1409,16 +1438,16 @@
       <c r="C1" s="1">
         <v>45320</v>
       </c>
-      <c r="D1" s="2">
+      <c r="D1">
         <f>COUNTIF(A1:B31,$A1)</f>
         <v>2</v>
       </c>
       <c r="E1" s="2">
-        <f>COUNT($A$1:$B$31) - D1</f>
-        <v>29</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+        <f>COUNT($A$1:$B$33) - D1</f>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
       <c r="A2" s="1">
         <v>45320</v>
       </c>
@@ -1428,16 +1457,16 @@
       <c r="C2" s="1">
         <v>45321</v>
       </c>
-      <c r="D2" s="2">
+      <c r="D2">
         <f>COUNTIF(A2:B32,"30.01.2024")</f>
         <v>5</v>
       </c>
-      <c r="E2" s="2">
+      <c r="E2">
         <f>E1 - D2</f>
-        <v>24</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
       <c r="A3" s="1">
         <v>45321</v>
       </c>
@@ -1447,16 +1476,16 @@
       <c r="C3" s="1">
         <v>45322</v>
       </c>
-      <c r="D3" s="2">
+      <c r="D3">
         <f>COUNTIF(A3:B33,"31.01.2024")</f>
         <v>4</v>
       </c>
-      <c r="E3" s="2">
-        <f t="shared" ref="E3:E11" si="0">E2 - D3</f>
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E3">
+        <f t="shared" ref="E3:E12" si="0">E2 - D3</f>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
       <c r="A4" s="1">
         <v>45321</v>
       </c>
@@ -1466,16 +1495,16 @@
       <c r="C4" s="1">
         <v>45323</v>
       </c>
-      <c r="D4" s="2">
+      <c r="D4">
         <f>COUNTIF(A4:B34,"01.02.2024")</f>
         <v>3</v>
       </c>
-      <c r="E4" s="2">
+      <c r="E4">
         <f t="shared" si="0"/>
-        <v>17</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
       <c r="A5" s="1">
         <v>45321</v>
       </c>
@@ -1485,35 +1514,35 @@
       <c r="C5" s="1">
         <v>45324</v>
       </c>
-      <c r="D5" s="2">
+      <c r="D5">
         <f>COUNTIF(A5:B35,"02.02.2024")</f>
         <v>1</v>
       </c>
-      <c r="E5" s="2">
+      <c r="E5">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="1">
+        <v>45321</v>
+      </c>
+      <c r="B6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="1">
+        <v>45329</v>
+      </c>
+      <c r="D6">
+        <f>COUNTIF(A6:B36,"07.02.2024")</f>
+        <v>2</v>
+      </c>
+      <c r="E6">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
-        <v>45321</v>
-      </c>
-      <c r="B6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" s="1">
-        <v>45329</v>
-      </c>
-      <c r="D6" s="2">
-        <f>COUNTIF(A6:B36,"07.02.2024")</f>
-        <v>2</v>
-      </c>
-      <c r="E6" s="2">
-        <f t="shared" si="0"/>
-        <v>14</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5">
       <c r="A7" s="1">
         <v>45321</v>
       </c>
@@ -1523,16 +1552,16 @@
       <c r="C7" s="1">
         <v>45339</v>
       </c>
-      <c r="D7" s="2">
+      <c r="D7">
         <f>COUNTIF(A7:B37,"17.02.2024")</f>
         <v>3</v>
       </c>
-      <c r="E7" s="2">
+      <c r="E7">
         <f t="shared" si="0"/>
-        <v>11</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
       <c r="A8" s="1">
         <v>45322</v>
       </c>
@@ -1542,16 +1571,16 @@
       <c r="C8" s="1">
         <v>45343</v>
       </c>
-      <c r="D8" s="2">
+      <c r="D8">
         <f>COUNTIF(A8:B38,"21.02.2024")</f>
         <v>3</v>
       </c>
-      <c r="E8" s="2">
+      <c r="E8">
         <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
       <c r="A9" s="1">
         <v>45322</v>
       </c>
@@ -1561,16 +1590,16 @@
       <c r="C9" s="1">
         <v>45348</v>
       </c>
-      <c r="D9" s="2">
+      <c r="D9">
         <f>COUNTIF(A9:B39,"26.02.2024")</f>
         <v>4</v>
       </c>
-      <c r="E9" s="2">
+      <c r="E9">
         <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
       <c r="A10" s="1">
         <v>45322</v>
       </c>
@@ -1580,16 +1609,16 @@
       <c r="C10" s="1">
         <v>45353</v>
       </c>
-      <c r="D10" s="2">
+      <c r="D10">
         <f>COUNTIF(A10:B40,"02.03.2024")</f>
         <v>3</v>
       </c>
-      <c r="E10" s="2">
+      <c r="E10">
         <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
       <c r="A11" s="1">
         <v>45322</v>
       </c>
@@ -1599,194 +1628,201 @@
       <c r="C11" s="1">
         <v>45362</v>
       </c>
-      <c r="D11" s="2">
+      <c r="D11">
         <f>COUNTIF(A11:B41,"11.03.2024")</f>
         <v>1</v>
       </c>
-      <c r="E11" s="2">
+      <c r="E11">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" s="1">
+        <v>45323</v>
+      </c>
+      <c r="B12" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" s="1">
+        <v>45365</v>
+      </c>
+      <c r="D12">
+        <f>COUNTIF(A12:B42,"14.03.2024")</f>
+        <v>2</v>
+      </c>
+      <c r="E12">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="1">
-        <v>45323</v>
-      </c>
-      <c r="B12" t="s">
-        <v>11</v>
-      </c>
-      <c r="D12" s="2"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5">
       <c r="A13" s="1">
         <v>45323</v>
       </c>
       <c r="B13" t="s">
         <v>12</v>
       </c>
-      <c r="D13" s="2"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:5">
       <c r="A14" s="1">
         <v>45323</v>
       </c>
       <c r="B14" t="s">
         <v>13</v>
       </c>
-      <c r="D14" s="2"/>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:5">
       <c r="A15" s="1">
         <v>45324</v>
       </c>
       <c r="B15" t="s">
         <v>14</v>
       </c>
-      <c r="D15" s="2"/>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:5">
       <c r="A16" s="1">
         <v>45329</v>
       </c>
       <c r="B16" t="s">
         <v>15</v>
       </c>
-      <c r="D16" s="2"/>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:2">
       <c r="A17" s="1">
         <v>45329</v>
       </c>
       <c r="B17" t="s">
         <v>16</v>
       </c>
-      <c r="D17" s="2"/>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:2">
       <c r="A18" s="1">
         <v>45339</v>
       </c>
       <c r="B18" t="s">
         <v>17</v>
       </c>
-      <c r="D18" s="2"/>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:2">
       <c r="A19" s="1">
         <v>45339</v>
       </c>
       <c r="B19" t="s">
         <v>18</v>
       </c>
-      <c r="D19" s="2"/>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:2">
       <c r="A20" s="1">
         <v>45339</v>
       </c>
       <c r="B20" t="s">
         <v>19</v>
       </c>
-      <c r="D20" s="2"/>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:2">
       <c r="A21" s="1">
         <v>45343</v>
       </c>
       <c r="B21" t="s">
         <v>20</v>
       </c>
-      <c r="D21" s="2"/>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:2">
       <c r="A22" s="1">
         <v>45343</v>
       </c>
       <c r="B22" t="s">
         <v>21</v>
       </c>
-      <c r="D22" s="2"/>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="1:2">
       <c r="A23" s="1">
         <v>45343</v>
       </c>
       <c r="B23" t="s">
         <v>22</v>
       </c>
-      <c r="D23" s="2"/>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="1:2">
       <c r="A24" s="1">
         <v>45348</v>
       </c>
       <c r="B24" t="s">
         <v>23</v>
       </c>
-      <c r="D24" s="2"/>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="1:2">
       <c r="A25" s="1">
         <v>45348</v>
       </c>
       <c r="B25" t="s">
         <v>24</v>
       </c>
-      <c r="D25" s="2"/>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="1:2">
       <c r="A26" s="1">
         <v>45348</v>
       </c>
       <c r="B26" t="s">
         <v>25</v>
       </c>
-      <c r="D26" s="2"/>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="27" spans="1:2">
       <c r="A27" s="1">
         <v>45348</v>
       </c>
       <c r="B27" t="s">
         <v>26</v>
       </c>
-      <c r="D27" s="2"/>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="1:2">
       <c r="A28" s="1">
         <v>45353</v>
       </c>
       <c r="B28" t="s">
         <v>27</v>
       </c>
-      <c r="D28" s="2"/>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="29" spans="1:2">
       <c r="A29" s="1">
         <v>45353</v>
       </c>
       <c r="B29" t="s">
         <v>28</v>
       </c>
-      <c r="D29" s="2"/>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="30" spans="1:2">
       <c r="A30" s="1">
         <v>45353</v>
       </c>
       <c r="B30" t="s">
         <v>29</v>
       </c>
-      <c r="D30" s="2"/>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="31" spans="1:2">
       <c r="A31" s="1">
         <v>45362</v>
       </c>
       <c r="B31" t="s">
         <v>30</v>
       </c>
-      <c r="D31" s="2"/>
+    </row>
+    <row r="32" spans="1:2">
+      <c r="A32" s="1">
+        <v>45365</v>
+      </c>
+      <c r="B32" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2">
+      <c r="A33" s="1">
+        <v>45365</v>
+      </c>
+      <c r="B33" t="s">
+        <v>32</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>